<commit_message>
change data file and fixed objective function
</commit_message>
<xml_diff>
--- a/VRP/data.xlsx
+++ b/VRP/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\OR_Programming\Operational-Research\VRP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C7F2D53-522A-4E35-B019-52EA1355DEBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D00C0AF8-EAAC-4040-A91E-EC826E39238B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="parameters" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
   <si>
     <t>hospital</t>
   </si>
@@ -90,6 +90,9 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>h0</t>
   </si>
 </sst>
 </file>
@@ -557,8 +560,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D21BB982-1506-49FC-B41B-7E4779036593}">
   <dimension ref="A2:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -644,8 +647,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCC49B8D-9D1E-4FC6-A41F-C13C824390DF}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -660,7 +663,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>100</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -668,7 +671,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>100</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -682,7 +685,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -706,126 +709,139 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="B2">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="C2">
-        <v>52</v>
-      </c>
-      <c r="D2" s="1">
-        <v>5.25</v>
-      </c>
-      <c r="E2" s="1">
-        <v>1.75</v>
+        <v>40</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="C3">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="D3" s="1">
-        <v>22.5</v>
+        <v>5.25</v>
       </c>
       <c r="E3" s="1">
-        <v>7.5</v>
+        <v>1.75</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C4">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c r="D4" s="1">
-        <v>12</v>
+        <v>22.5</v>
       </c>
       <c r="E4" s="1">
-        <v>4</v>
+        <v>7.5</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5">
-        <v>20</v>
+        <v>52</v>
       </c>
       <c r="C5">
-        <v>26</v>
+        <v>64</v>
       </c>
       <c r="D5" s="1">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="E5" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="C6">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D6" s="1">
-        <v>15.75</v>
+        <v>6</v>
       </c>
       <c r="E6" s="1">
-        <v>5.25</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="C7">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="D7" s="1">
-        <v>11.25</v>
+        <v>15.75</v>
       </c>
       <c r="E7" s="1">
-        <v>3.75</v>
+        <v>5.25</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <v>21</v>
+      </c>
+      <c r="C8">
+        <v>47</v>
+      </c>
+      <c r="D8" s="1">
+        <v>11.25</v>
+      </c>
+      <c r="E8" s="1">
+        <v>3.75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>9</v>
       </c>
-      <c r="B8">
+      <c r="B9">
         <v>17</v>
       </c>
-      <c r="C8">
+      <c r="C9">
         <v>63</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D9" s="1">
         <v>14.25</v>
       </c>
-      <c r="E8" s="1">
+      <c r="E9" s="1">
         <v>4.75</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fix data and MIP model
data: k: 2-->3
MIP model: Fix constraints and objective. Add print result
</commit_message>
<xml_diff>
--- a/VRP/data.xlsx
+++ b/VRP/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\OR_Programming\Operational-Research\VRP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dave\Documents\GitHub\Operational-Research\VRP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D00C0AF8-EAAC-4040-A91E-EC826E39238B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{305C45C6-376D-424A-9313-56601AB38000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="parameters" sheetId="2" r:id="rId1"/>
@@ -243,6 +243,50 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>91440</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>53340</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>25862</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>26768</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3020A467-7A8E-1877-01B8-9039EE75987F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="91440" y="2796540"/>
+          <a:ext cx="7859222" cy="704948"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -250,23 +294,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>561975</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>68580</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>352991</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>181246</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>517338</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>61364</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
+        <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{875B7D6C-D6CF-41D1-873A-75541C0BE4A8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D659A7D0-C2E6-DCAE-8AE4-648C089FC946}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -282,8 +326,52 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4829175" y="142875"/>
-          <a:ext cx="4058216" cy="1943371"/>
+          <a:off x="3116580" y="1005840"/>
+          <a:ext cx="7763958" cy="2896004"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>135255</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>59055</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>403013</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>5784</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8924050E-16EB-D92C-0516-8DEE7D98500B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3792855" y="790575"/>
+          <a:ext cx="7582958" cy="495369"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -560,13 +648,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D21BB982-1506-49FC-B41B-7E4779036593}">
   <dimension ref="A2:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -583,7 +671,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -600,12 +688,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>15</v>
       </c>
       <c r="B4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D4" t="s">
         <v>14</v>
@@ -617,7 +705,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -647,18 +735,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCC49B8D-9D1E-4FC6-A41F-C13C824390DF}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -666,7 +754,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -685,12 +773,12 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -707,7 +795,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -724,7 +812,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -741,7 +829,7 @@
         <v>1.75</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -758,7 +846,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -775,7 +863,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -792,7 +880,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -809,7 +897,7 @@
         <v>5.25</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -826,7 +914,7 @@
         <v>3.75</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>9</v>
       </c>

</xml_diff>

<commit_message>
initialize population with size 50
</commit_message>
<xml_diff>
--- a/VRP/data.xlsx
+++ b/VRP/data.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dave\Documents\GitHub\Operational-Research\VRP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\OR_Programming\Operational-Research\VRP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{305C45C6-376D-424A-9313-56601AB38000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3D014F3-3E08-4FBC-B839-42D5C676E26A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="parameters" sheetId="2" r:id="rId1"/>
     <sheet name="capacity" sheetId="3" r:id="rId2"/>
     <sheet name="coor" sheetId="1" r:id="rId3"/>
+    <sheet name="test" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
   <si>
     <t>hospital</t>
   </si>
@@ -93,6 +94,12 @@
   </si>
   <si>
     <t>h0</t>
+  </si>
+  <si>
+    <t>q1</t>
+  </si>
+  <si>
+    <t>q2</t>
   </si>
 </sst>
 </file>
@@ -108,12 +115,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -128,9 +141,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -648,13 +662,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D21BB982-1506-49FC-B41B-7E4779036593}">
   <dimension ref="A2:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -671,7 +685,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -688,7 +702,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -705,7 +719,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -739,14 +753,14 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -754,7 +768,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -773,12 +787,12 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D3" sqref="D3:E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -795,7 +809,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -812,7 +826,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -829,7 +843,7 @@
         <v>1.75</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -846,7 +860,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -863,7 +877,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -880,7 +894,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -897,7 +911,7 @@
         <v>5.25</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -914,7 +928,7 @@
         <v>3.75</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -935,4 +949,140 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70C3919D-2DBE-49F2-AA14-6E3A7FDF3263}">
+  <dimension ref="A1:C11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8:F9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>5.25</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1.75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>22.5</v>
+      </c>
+      <c r="C3" s="1">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
+        <v>12</v>
+      </c>
+      <c r="C4" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1">
+        <v>6</v>
+      </c>
+      <c r="C5" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1">
+        <v>15.75</v>
+      </c>
+      <c r="C6" s="1">
+        <v>5.25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1">
+        <v>11.25</v>
+      </c>
+      <c r="C7" s="1">
+        <v>3.75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1">
+        <v>14.25</v>
+      </c>
+      <c r="C8" s="1">
+        <v>4.75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2">
+        <v>5.25</v>
+      </c>
+      <c r="C9" s="2">
+        <v>1.75</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2">
+        <v>22.5</v>
+      </c>
+      <c r="C10" s="2">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2">
+        <v>12</v>
+      </c>
+      <c r="C11" s="2">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
mai fix tiep', ditt mm
</commit_message>
<xml_diff>
--- a/VRP/data.xlsx
+++ b/VRP/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\OR_Programming\Operational-Research\VRP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3D014F3-3E08-4FBC-B839-42D5C676E26A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C69697F5-8086-4C3A-B2F0-0C6912868613}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="parameters" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="21">
   <si>
     <t>hospital</t>
   </si>
@@ -784,10 +784,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3:E9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -943,6 +943,68 @@
       </c>
       <c r="E9" s="1">
         <v>4.75</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13">
+        <f>VLOOKUP(B13,$A$1:$E$9,4,)</f>
+        <v>11.25</v>
+      </c>
+      <c r="D13">
+        <f>VLOOKUP(B13,$A$1:$E$9,5,)</f>
+        <v>3.75</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14">
+        <f t="shared" ref="C14:C17" si="0">VLOOKUP(B14,$A$1:$E$9,4,)</f>
+        <v>12</v>
+      </c>
+      <c r="D14">
+        <f t="shared" ref="D14:D16" si="1">VLOOKUP(B14,$A$1:$E$9,5,)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="0"/>
+        <v>22.5</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="1"/>
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="0"/>
+        <v>14.25</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="1"/>
+        <v>4.75</v>
+      </c>
+    </row>
+    <row r="17" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C17">
+        <f>SUM(C13:C16)</f>
+        <v>60</v>
+      </c>
+      <c r="D17">
+        <f>SUM(D13:D16)</f>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -955,7 +1017,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70C3919D-2DBE-49F2-AA14-6E3A7FDF3263}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F8" sqref="F8:F9"/>
     </sheetView>
   </sheetViews>

</xml_diff>